<commit_message>
Cambios en grafica e integacuín modulo 1 y 3
</commit_message>
<xml_diff>
--- a/Parte1/Datos/annual_savings.xlsx
+++ b/Parte1/Datos/annual_savings.xlsx
@@ -408,13 +408,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>679.09173432</v>
+        <v>1161.56531337</v>
       </c>
       <c r="C2">
-        <v>745.8028921775</v>
+        <v>1290.366832755</v>
       </c>
       <c r="D2">
-        <v>654.392780525</v>
+        <v>1128.38323257</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -422,13 +422,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>771.0029565049999</v>
+        <v>1318.93042116</v>
       </c>
       <c r="C3">
-        <v>852.8367052475</v>
+        <v>1476.90389847</v>
       </c>
       <c r="D3">
-        <v>755.7196542775</v>
+        <v>1304.22379527</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -436,13 +436,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1077.29482608</v>
+        <v>1838.26286061</v>
       </c>
       <c r="C4">
-        <v>1181.119627125</v>
+        <v>2037.872878195</v>
       </c>
       <c r="D4">
-        <v>1032.58971115</v>
+        <v>1774.65915594</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -450,13 +450,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1037.46010299</v>
+        <v>1740.92691168</v>
       </c>
       <c r="C5">
-        <v>1139.47489194</v>
+        <v>1934.319344265</v>
       </c>
       <c r="D5">
-        <v>1000.3554035475</v>
+        <v>1693.155997665</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -464,13 +464,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>980.0653262849999</v>
+        <v>1614.08635509</v>
       </c>
       <c r="C6">
-        <v>1076.4330720025</v>
+        <v>1793.372514395</v>
       </c>
       <c r="D6">
-        <v>945.00637362</v>
+        <v>1569.74176161</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>925.9019645249999</v>
+        <v>1496.48059374</v>
       </c>
       <c r="C7">
-        <v>1016.953406975</v>
+        <v>1662.69101383</v>
       </c>
       <c r="D7">
-        <v>892.7986128975</v>
+        <v>1455.3419562</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>874.7494862999999</v>
+        <v>1387.73169942</v>
       </c>
       <c r="C8">
-        <v>960.7694647549999</v>
+        <v>1541.87615736</v>
       </c>
       <c r="D8">
-        <v>843.4772359875001</v>
+        <v>1349.60810787</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>826.30058506</v>
+        <v>1286.56100265</v>
       </c>
       <c r="C9">
-        <v>907.5520575475</v>
+        <v>1429.48568917</v>
       </c>
       <c r="D9">
-        <v>796.7533114125</v>
+        <v>1251.235521855</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -520,13 +520,13 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>780.5661798199999</v>
+        <v>1192.73770539</v>
       </c>
       <c r="C10">
-        <v>857.3215119475001</v>
+        <v>1325.236894905</v>
       </c>
       <c r="D10">
-        <v>752.6555996075</v>
+        <v>1159.980749235</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -534,13 +534,13 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>737.410060555</v>
+        <v>1105.9239444</v>
       </c>
       <c r="C11">
-        <v>809.9277825825</v>
+        <v>1228.773574875</v>
       </c>
       <c r="D11">
-        <v>711.059123155</v>
+        <v>1075.549397175</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -548,13 +548,13 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>696.600647355</v>
+        <v>1025.20965129</v>
       </c>
       <c r="C12">
-        <v>765.1009588325001</v>
+        <v>1139.07572471</v>
       </c>
       <c r="D12">
-        <v>671.681747855</v>
+        <v>997.020076635</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -562,13 +562,13 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>677.2416698249999</v>
+        <v>985.78139979</v>
       </c>
       <c r="C13">
-        <v>743.743980415</v>
+        <v>1095.045481145</v>
       </c>
       <c r="D13">
-        <v>652.4778294450001</v>
+        <v>957.4192232550001</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -576,13 +576,13 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>674.2663714199999</v>
+        <v>977.8035728999999</v>
       </c>
       <c r="C14">
-        <v>740.4810133225001</v>
+        <v>1086.19635971</v>
       </c>
       <c r="D14">
-        <v>649.6111316700001</v>
+        <v>949.7120138550001</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -590,13 +590,13 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>671.7555077249999</v>
+        <v>970.11390432</v>
       </c>
       <c r="C15">
-        <v>737.72680238</v>
+        <v>1077.63008969</v>
       </c>
       <c r="D15">
-        <v>647.2150583625</v>
+        <v>942.204296385</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -604,13 +604,13 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>668.908468385</v>
+        <v>962.4954292799999</v>
       </c>
       <c r="C16">
-        <v>734.6004592975</v>
+        <v>1069.2015873</v>
       </c>
       <c r="D16">
-        <v>644.46447575</v>
+        <v>934.86753063</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -618,13 +618,13 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>666.33371482</v>
+        <v>954.5737789499999</v>
       </c>
       <c r="C17">
-        <v>731.7694395225</v>
+        <v>1060.379130195</v>
       </c>
       <c r="D17">
-        <v>641.96894072</v>
+        <v>927.112512645</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -632,13 +632,13 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>663.524503485</v>
+        <v>947.0004030299999</v>
       </c>
       <c r="C18">
-        <v>728.6968480025</v>
+        <v>1052.01493936</v>
       </c>
       <c r="D18">
-        <v>639.3132921175001</v>
+        <v>919.89609426</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -646,13 +646,13 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>660.946878415</v>
+        <v>939.46930077</v>
       </c>
       <c r="C19">
-        <v>725.8451063825</v>
+        <v>1043.573234935</v>
       </c>
       <c r="D19">
-        <v>636.7665346825</v>
+        <v>912.3845083650001</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -660,13 +660,13 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>658.230534435</v>
+        <v>932.0807126399999</v>
       </c>
       <c r="C20">
-        <v>722.86489362</v>
+        <v>1035.41694872</v>
       </c>
       <c r="D20">
-        <v>634.1552392975</v>
+        <v>905.328139815</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -674,13 +674,13 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>655.62462841</v>
+        <v>924.3897874199999</v>
       </c>
       <c r="C21">
-        <v>720.0088148925</v>
+        <v>1026.857358065</v>
       </c>
       <c r="D21">
-        <v>631.6519829375001</v>
+        <v>897.8312118600001</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -688,13 +688,13 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>653.047067195</v>
+        <v>917.0888007599999</v>
       </c>
       <c r="C22">
-        <v>717.173680325</v>
+        <v>1018.75616689</v>
       </c>
       <c r="D22">
-        <v>629.1691470475</v>
+        <v>890.76821724</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -702,13 +702,13 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>650.270637385</v>
+        <v>909.79125369</v>
       </c>
       <c r="C23">
-        <v>714.124629495</v>
+        <v>1010.62405906</v>
       </c>
       <c r="D23">
-        <v>626.4943802150001</v>
+        <v>883.59581475</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -716,13 +716,13 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>647.7887106549999</v>
+        <v>902.50135932</v>
       </c>
       <c r="C24">
-        <v>711.3983349800001</v>
+        <v>1002.54305998</v>
       </c>
       <c r="D24">
-        <v>624.10071836</v>
+        <v>876.560725755</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -730,13 +730,13 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>645.013834805</v>
+        <v>895.20702579</v>
       </c>
       <c r="C25">
-        <v>708.3704720125</v>
+        <v>994.468441505</v>
       </c>
       <c r="D25">
-        <v>621.468658485</v>
+        <v>869.5521058950001</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -744,13 +744,13 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>642.5357450199999</v>
+        <v>888.1406522999999</v>
       </c>
       <c r="C26">
-        <v>705.6347181225001</v>
+        <v>986.5680782650001</v>
       </c>
       <c r="D26">
-        <v>619.04236787</v>
+        <v>862.57529028</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -758,13 +758,13 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>639.985424255</v>
+        <v>881.0896142399999</v>
       </c>
       <c r="C27">
-        <v>702.82827388</v>
+        <v>978.7516457950001</v>
       </c>
       <c r="D27">
-        <v>616.5782001125</v>
+        <v>855.7481765250001</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -772,13 +772,13 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>637.3795182299999</v>
+        <v>873.8985614699999</v>
       </c>
       <c r="C28">
-        <v>699.9721951525</v>
+        <v>970.801453545</v>
       </c>
       <c r="D28">
-        <v>614.0749437525</v>
+        <v>848.85102621</v>
       </c>
     </row>
   </sheetData>

</xml_diff>